<commit_message>
Code and readme development. Nearly stable cube
</commit_message>
<xml_diff>
--- a/MotorData.xlsx
+++ b/MotorData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark\Documents\GitHub\Cube\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6CC4932-3324-46B1-8136-B932D6456795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E475622F-A623-40B2-A507-490DFFFA9955}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{EC7B1352-56D2-4F86-A349-4A1459A01683}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{EC7B1352-56D2-4F86-A349-4A1459A01683}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3400,6 +3400,20 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet2!$D$2:$D$465</c:f>
@@ -3407,451 +3421,451 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="464"/>
                 <c:pt idx="0">
-                  <c:v>1.0509999999999999</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.151</c:v>
+                  <c:v>0.10000000000000009</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.2509999999999999</c:v>
+                  <c:v>0.19999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.351</c:v>
+                  <c:v>0.30000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.4510000000000001</c:v>
+                  <c:v>0.40000000000000013</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.5509999999999999</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.651</c:v>
+                  <c:v>0.60000000000000009</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.7509999999999999</c:v>
+                  <c:v>0.7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.851</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.9510000000000001</c:v>
+                  <c:v>0.90000000000000013</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.0510000000000002</c:v>
+                  <c:v>1.0000000000000002</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.1509999999999998</c:v>
+                  <c:v>1.0999999999999999</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.2509999999999999</c:v>
+                  <c:v>1.2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.351</c:v>
+                  <c:v>1.3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.4510000000000001</c:v>
+                  <c:v>1.4000000000000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.5510000000000002</c:v>
+                  <c:v>1.5000000000000002</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.6509999999999998</c:v>
+                  <c:v>1.5999999999999999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.7509999999999999</c:v>
+                  <c:v>1.7</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.851</c:v>
+                  <c:v>1.8</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.9510000000000001</c:v>
+                  <c:v>1.9000000000000001</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>3.0510000000000002</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>3.1509999999999998</c:v>
+                  <c:v>2.0999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>3.2509999999999999</c:v>
+                  <c:v>2.2000000000000002</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>3.351</c:v>
+                  <c:v>2.2999999999999998</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3.4510000000000001</c:v>
+                  <c:v>2.4000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>3.5510000000000002</c:v>
+                  <c:v>2.5</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>3.6509999999999998</c:v>
+                  <c:v>2.5999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>3.7509999999999999</c:v>
+                  <c:v>2.7</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>3.851</c:v>
+                  <c:v>2.8</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>3.9510000000000001</c:v>
+                  <c:v>2.9000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>4.0510000000000002</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>4.1509999999999998</c:v>
+                  <c:v>3.0999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>4.2510000000000003</c:v>
+                  <c:v>3.2</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>4.351</c:v>
+                  <c:v>3.3</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>4.4509999999999996</c:v>
+                  <c:v>3.3999999999999995</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>4.5510000000000002</c:v>
+                  <c:v>3.5</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>4.6509999999999998</c:v>
+                  <c:v>3.5999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>4.7510000000000003</c:v>
+                  <c:v>3.7</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>4.851</c:v>
+                  <c:v>3.8</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>4.9509999999999996</c:v>
+                  <c:v>3.8999999999999995</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>5.0510000000000002</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>5.1509999999999998</c:v>
+                  <c:v>4.0999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>5.2510000000000003</c:v>
+                  <c:v>4.2</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>5.351</c:v>
+                  <c:v>4.3</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>5.4509999999999996</c:v>
+                  <c:v>4.3999999999999995</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>5.5510000000000002</c:v>
+                  <c:v>4.5</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>5.6509999999999998</c:v>
+                  <c:v>4.5999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>5.7510000000000003</c:v>
+                  <c:v>4.7</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>5.851</c:v>
+                  <c:v>4.8</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>5.9509999999999996</c:v>
+                  <c:v>4.8999999999999995</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>6.0510000000000002</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>6.1509999999999998</c:v>
+                  <c:v>5.0999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>6.2510000000000003</c:v>
+                  <c:v>5.2</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>6.351</c:v>
+                  <c:v>5.3</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>6.4509999999999996</c:v>
+                  <c:v>5.3999999999999995</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>6.5510000000000002</c:v>
+                  <c:v>5.5</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>6.6509999999999998</c:v>
+                  <c:v>5.6</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>6.7510000000000003</c:v>
+                  <c:v>5.7</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>6.851</c:v>
+                  <c:v>5.8</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>6.9509999999999996</c:v>
+                  <c:v>5.8999999999999995</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>7.0510000000000002</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>7.1509999999999998</c:v>
+                  <c:v>6.1</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>7.2510000000000003</c:v>
+                  <c:v>6.2</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>7.351</c:v>
+                  <c:v>6.3</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>7.4509999999999996</c:v>
+                  <c:v>6.3999999999999995</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>7.5510000000000002</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>7.6509999999999998</c:v>
+                  <c:v>6.6</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>7.7510000000000003</c:v>
+                  <c:v>6.7</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>7.851</c:v>
+                  <c:v>6.8</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>7.9509999999999996</c:v>
+                  <c:v>6.8999999999999995</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>8.0510000000000002</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>8.1509999999999998</c:v>
+                  <c:v>7.1</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>8.2509999999999994</c:v>
+                  <c:v>7.1999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>8.3510000000000009</c:v>
+                  <c:v>7.3000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>8.4510000000000005</c:v>
+                  <c:v>7.4</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>8.5510000000000002</c:v>
+                  <c:v>7.5</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>8.6509999999999998</c:v>
+                  <c:v>7.6</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>8.7509999999999994</c:v>
+                  <c:v>7.6999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>8.8510000000000009</c:v>
+                  <c:v>7.8000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>8.9510000000000005</c:v>
+                  <c:v>7.9</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>9.0510000000000002</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>9.1509999999999998</c:v>
+                  <c:v>8.1</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>9.2509999999999994</c:v>
+                  <c:v>8.1999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>9.3510000000000009</c:v>
+                  <c:v>8.3000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>9.4510000000000005</c:v>
+                  <c:v>8.4</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>9.5510000000000002</c:v>
+                  <c:v>8.5</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>9.6509999999999998</c:v>
+                  <c:v>8.6</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>9.7509999999999994</c:v>
+                  <c:v>8.6999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>9.8510000000000009</c:v>
+                  <c:v>8.8000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>9.9510000000000005</c:v>
+                  <c:v>8.9</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>10.051</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>10.151</c:v>
+                  <c:v>9.1</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>10.250999999999999</c:v>
+                  <c:v>9.1999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>10.351000000000001</c:v>
+                  <c:v>9.3000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>10.451000000000001</c:v>
+                  <c:v>9.4</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>10.551</c:v>
+                  <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>10.651</c:v>
+                  <c:v>9.6</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>10.750999999999999</c:v>
+                  <c:v>9.6999999999999993</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>10.851000000000001</c:v>
+                  <c:v>9.8000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>10.951000000000001</c:v>
+                  <c:v>9.9</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>11.051</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>11.151</c:v>
+                  <c:v>10.1</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>11.250999999999999</c:v>
+                  <c:v>10.199999999999999</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>11.351000000000001</c:v>
+                  <c:v>10.3</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>11.451000000000001</c:v>
+                  <c:v>10.4</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>11.551</c:v>
+                  <c:v>10.5</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>11.651</c:v>
+                  <c:v>10.6</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>11.750999999999999</c:v>
+                  <c:v>10.7</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>11.851000000000001</c:v>
+                  <c:v>10.8</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>11.951000000000001</c:v>
+                  <c:v>10.9</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>12.051</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>12.151</c:v>
+                  <c:v>11.1</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>12.250999999999999</c:v>
+                  <c:v>11.2</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>12.351000000000001</c:v>
+                  <c:v>11.3</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>12.451000000000001</c:v>
+                  <c:v>11.4</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>12.551</c:v>
+                  <c:v>11.5</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>12.651</c:v>
+                  <c:v>11.6</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>12.750999999999999</c:v>
+                  <c:v>11.7</c:v>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>12.851000000000001</c:v>
+                  <c:v>11.8</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>12.951000000000001</c:v>
+                  <c:v>11.9</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>13.051</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>13.151</c:v>
+                  <c:v>12.1</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>13.250999999999999</c:v>
+                  <c:v>12.2</c:v>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>13.351000000000001</c:v>
+                  <c:v>12.3</c:v>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>13.451000000000001</c:v>
+                  <c:v>12.4</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>13.551</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>13.651</c:v>
+                  <c:v>12.6</c:v>
                 </c:pt>
                 <c:pt idx="127">
-                  <c:v>13.750999999999999</c:v>
+                  <c:v>12.7</c:v>
                 </c:pt>
                 <c:pt idx="128">
-                  <c:v>13.851000000000001</c:v>
+                  <c:v>12.8</c:v>
                 </c:pt>
                 <c:pt idx="129">
-                  <c:v>13.951000000000001</c:v>
+                  <c:v>12.9</c:v>
                 </c:pt>
                 <c:pt idx="130">
-                  <c:v>14.051</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="131">
-                  <c:v>14.151</c:v>
+                  <c:v>13.1</c:v>
                 </c:pt>
                 <c:pt idx="132">
-                  <c:v>14.250999999999999</c:v>
+                  <c:v>13.2</c:v>
                 </c:pt>
                 <c:pt idx="133">
-                  <c:v>14.351000000000001</c:v>
+                  <c:v>13.3</c:v>
                 </c:pt>
                 <c:pt idx="134">
-                  <c:v>14.451000000000001</c:v>
+                  <c:v>13.4</c:v>
                 </c:pt>
                 <c:pt idx="135">
-                  <c:v>14.551</c:v>
+                  <c:v>13.5</c:v>
                 </c:pt>
                 <c:pt idx="136">
-                  <c:v>14.651</c:v>
+                  <c:v>13.6</c:v>
                 </c:pt>
                 <c:pt idx="137">
-                  <c:v>14.750999999999999</c:v>
+                  <c:v>13.7</c:v>
                 </c:pt>
                 <c:pt idx="138">
-                  <c:v>14.851000000000001</c:v>
+                  <c:v>13.8</c:v>
                 </c:pt>
                 <c:pt idx="139">
-                  <c:v>14.951000000000001</c:v>
+                  <c:v>13.9</c:v>
                 </c:pt>
                 <c:pt idx="140">
-                  <c:v>15.051</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="141">
-                  <c:v>15.151</c:v>
+                  <c:v>14.1</c:v>
                 </c:pt>
                 <c:pt idx="142">
-                  <c:v>15.250999999999999</c:v>
+                  <c:v>14.2</c:v>
                 </c:pt>
                 <c:pt idx="143">
-                  <c:v>15.351000000000001</c:v>
+                  <c:v>14.3</c:v>
                 </c:pt>
                 <c:pt idx="144">
-                  <c:v>15.451000000000001</c:v>
+                  <c:v>14.4</c:v>
                 </c:pt>
                 <c:pt idx="145">
-                  <c:v>15.551</c:v>
+                  <c:v>14.5</c:v>
                 </c:pt>
                 <c:pt idx="146">
-                  <c:v>15.651</c:v>
+                  <c:v>14.6</c:v>
                 </c:pt>
                 <c:pt idx="147">
-                  <c:v>15.750999999999999</c:v>
+                  <c:v>14.7</c:v>
                 </c:pt>
                 <c:pt idx="148">
-                  <c:v>15.851000000000001</c:v>
+                  <c:v>14.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4316,6 +4330,595 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-EFB0-4D78-A2C6-88201EB7C32C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Approx Eqn</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$D$2:$D$92</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="91"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.10000000000000009</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.19999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.30000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.40000000000000013</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.60000000000000009</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.90000000000000013</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.0000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0999999999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.4000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.5000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.5999999999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.9000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.5999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2.9000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3.3</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3.3999999999999995</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3.5999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3.7</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>3.8</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>3.8999999999999995</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>4.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>4.3</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>4.3999999999999995</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4.5999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>4.7</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>4.8999999999999995</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>5.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>5.2</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>5.3</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>5.3999999999999995</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>5.6</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>5.7</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>5.8</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>5.8999999999999995</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>6.1</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>6.2</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>6.3</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>6.3999999999999995</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>6.5</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>6.6</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>6.7</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>6.8</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>6.8999999999999995</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>7.1</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>7.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>7.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>7.4</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>7.6</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>7.6999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>7.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>7.9</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>8.1</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>8.1999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>8.3000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>8.4</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>8.6</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>8.6999999999999993</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>8.8000000000000007</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>8.9</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$E$2:$E$92</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="91"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.2674130677869373</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.25089028037321</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.9751054601975486</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11.46258829220216</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>13.733910647845402</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>15.807856717691163</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>17.701578359598106</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>19.430736947262563</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>21.009632892224605</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>22.451323910504602</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>23.767733011953769</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>24.969747105407496</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>26.067307035121466</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>27.069489793106001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>27.984583587267416</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>28.820156386181658</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>29.583118507376224</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>30.279779766735217</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>30.915901661662019</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>31.49674501956251</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>32.027113505709238</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>32.511393350303365</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>32.953589623283314</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>33.357359356878661</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>33.726041789837666</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>34.062685983453221</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>34.370076037775853</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>34.650754116555888</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>34.907041471334665</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>35.141057638557257</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>35.354737968469834</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>35.549849630768442</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>35.728006229368319</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>35.890681147160279</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>36.039219731117278</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>36.17485041852396</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>36.298694896344863</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>36.411777377750731</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>36.515033072521405</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>36.609315921376727</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>36.695405658199661</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>36.774014258557223</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>36.845791827849666</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>36.911331977783597</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>36.971176735633513</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>37.025821026892011</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>37.075716768380879</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>37.121276605673806</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>37.162877325739672</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>37.200862973029679</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>37.235547694778624</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>37.267218339051638</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>37.296136827022451</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>37.322542319102403</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>37.346653192834388</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>37.368668848909259</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>37.388771360240639</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>37.407126977736404</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>37.423887505219582</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>37.439191554869744</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>37.453165693567328</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>37.465925489621519</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>37.477576468538217</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>37.488214985732441</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>37.497929023402669</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>37.506798918157344</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>37.514898025411192</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>37.522293326045926</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>37.52904598035262</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>37.535211833836868</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>37.540841879069831</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>37.545982677404751</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>37.550676744046633</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>37.554962899659607</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>37.55887659141991</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>37.562450186169556</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>37.565713238095157</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>37.568692733145689</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>37.571413312210481</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>37.573897474903255</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>37.576165765637384</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>37.578236943531458</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>37.580128137550084</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>37.581854988163123</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>37.583431776694795</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>37.584871543432492</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>37.586186195471967</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>37.587386605190865</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>37.588482700165031</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>37.589483545271051</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-8F83-4B75-B0D2-7AAA2B2EEA60}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -10044,16 +10647,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -17846,10 +18449,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95588423-1919-4188-9DF0-1F3766B91E31}">
-  <dimension ref="A1:D150"/>
+  <dimension ref="A1:G150"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17857,7 +18460,7 @@
     <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -17870,8 +18473,15 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F1">
+        <f>1.1</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G1">
+        <v>37.6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -17883,11 +18493,15 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <f>B2/1000</f>
-        <v>1.0509999999999999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <f>B2/1000 - 1.051</f>
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <f>$G$1*(1-EXP(-D2/$F$1))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>43</v>
       </c>
@@ -17899,11 +18513,15 @@
         <v>2.15</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D66" si="1">B3/1000</f>
-        <v>1.151</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" ref="D3:D66" si="1">B3/1000 - 1.051</f>
+        <v>0.10000000000000009</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E66" si="2">$G$1*(1-EXP(-D3/$F$1))</f>
+        <v>3.2674130677869373</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>125</v>
       </c>
@@ -17916,10 +18534,14 @@
       </c>
       <c r="D4">
         <f t="shared" si="1"/>
-        <v>1.2509999999999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="2"/>
+        <v>6.25089028037321</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>195</v>
       </c>
@@ -17932,10 +18554,14 @@
       </c>
       <c r="D5">
         <f t="shared" si="1"/>
-        <v>1.351</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="2"/>
+        <v>8.9751054601975486</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>254</v>
       </c>
@@ -17948,10 +18574,14 @@
       </c>
       <c r="D6">
         <f t="shared" si="1"/>
-        <v>1.4510000000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.40000000000000013</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="2"/>
+        <v>11.46258829220216</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>306</v>
       </c>
@@ -17964,10 +18594,14 @@
       </c>
       <c r="D7">
         <f t="shared" si="1"/>
-        <v>1.5509999999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.5</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="2"/>
+        <v>13.733910647845402</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>350</v>
       </c>
@@ -17980,10 +18614,14 @@
       </c>
       <c r="D8">
         <f t="shared" si="1"/>
-        <v>1.651</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.60000000000000009</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="2"/>
+        <v>15.807856717691163</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>389</v>
       </c>
@@ -17996,10 +18634,14 @@
       </c>
       <c r="D9">
         <f t="shared" si="1"/>
-        <v>1.7509999999999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.7</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="2"/>
+        <v>17.701578359598106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>423</v>
       </c>
@@ -18012,10 +18654,14 @@
       </c>
       <c r="D10">
         <f t="shared" si="1"/>
-        <v>1.851</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.8</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="2"/>
+        <v>19.430736947262563</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>453</v>
       </c>
@@ -18028,10 +18674,14 @@
       </c>
       <c r="D11">
         <f t="shared" si="1"/>
-        <v>1.9510000000000001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.90000000000000013</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="2"/>
+        <v>21.009632892224605</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>480</v>
       </c>
@@ -18044,10 +18694,14 @@
       </c>
       <c r="D12">
         <f t="shared" si="1"/>
-        <v>2.0510000000000002</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.0000000000000002</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="2"/>
+        <v>22.451323910504602</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>504</v>
       </c>
@@ -18060,10 +18714,14 @@
       </c>
       <c r="D13">
         <f t="shared" si="1"/>
-        <v>2.1509999999999998</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.0999999999999999</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="2"/>
+        <v>23.767733011953769</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>526</v>
       </c>
@@ -18076,10 +18734,14 @@
       </c>
       <c r="D14">
         <f t="shared" si="1"/>
-        <v>2.2509999999999999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.2</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="2"/>
+        <v>24.969747105407496</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>544</v>
       </c>
@@ -18092,10 +18754,14 @@
       </c>
       <c r="D15">
         <f t="shared" si="1"/>
-        <v>2.351</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.3</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="2"/>
+        <v>26.067307035121466</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>563</v>
       </c>
@@ -18108,10 +18774,14 @@
       </c>
       <c r="D16">
         <f t="shared" si="1"/>
-        <v>2.4510000000000001</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.4000000000000001</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="2"/>
+        <v>27.069489793106001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>578</v>
       </c>
@@ -18124,10 +18794,14 @@
       </c>
       <c r="D17">
         <f t="shared" si="1"/>
-        <v>2.5510000000000002</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.5000000000000002</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="2"/>
+        <v>27.984583587267416</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>592</v>
       </c>
@@ -18140,10 +18814,14 @@
       </c>
       <c r="D18">
         <f t="shared" si="1"/>
-        <v>2.6509999999999998</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.5999999999999999</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="2"/>
+        <v>28.820156386181658</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>605</v>
       </c>
@@ -18156,10 +18834,14 @@
       </c>
       <c r="D19">
         <f t="shared" si="1"/>
-        <v>2.7509999999999999</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.7</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="2"/>
+        <v>29.583118507376224</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>617</v>
       </c>
@@ -18172,10 +18854,14 @@
       </c>
       <c r="D20">
         <f t="shared" si="1"/>
-        <v>2.851</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.8</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="2"/>
+        <v>30.279779766735217</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>628</v>
       </c>
@@ -18188,10 +18874,14 @@
       </c>
       <c r="D21">
         <f t="shared" si="1"/>
-        <v>2.9510000000000001</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>1.9000000000000001</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="2"/>
+        <v>30.915901661662019</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>637</v>
       </c>
@@ -18204,10 +18894,14 @@
       </c>
       <c r="D22">
         <f t="shared" si="1"/>
-        <v>3.0510000000000002</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="2"/>
+        <v>31.49674501956251</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>647</v>
       </c>
@@ -18220,10 +18914,14 @@
       </c>
       <c r="D23">
         <f t="shared" si="1"/>
-        <v>3.1509999999999998</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2.0999999999999996</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="2"/>
+        <v>32.027113505709238</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>654</v>
       </c>
@@ -18236,10 +18934,14 @@
       </c>
       <c r="D24">
         <f t="shared" si="1"/>
-        <v>3.2509999999999999</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="2"/>
+        <v>32.511393350303365</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>663</v>
       </c>
@@ -18252,10 +18954,14 @@
       </c>
       <c r="D25">
         <f t="shared" si="1"/>
-        <v>3.351</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="2"/>
+        <v>32.953589623283314</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>668</v>
       </c>
@@ -18268,10 +18974,14 @@
       </c>
       <c r="D26">
         <f t="shared" si="1"/>
-        <v>3.4510000000000001</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2.4000000000000004</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="2"/>
+        <v>33.357359356878661</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>675</v>
       </c>
@@ -18284,10 +18994,14 @@
       </c>
       <c r="D27">
         <f t="shared" si="1"/>
-        <v>3.5510000000000002</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2.5</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="2"/>
+        <v>33.726041789837666</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>681</v>
       </c>
@@ -18300,10 +19014,14 @@
       </c>
       <c r="D28">
         <f t="shared" si="1"/>
-        <v>3.6509999999999998</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2.5999999999999996</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="2"/>
+        <v>34.062685983453221</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>687</v>
       </c>
@@ -18316,10 +19034,14 @@
       </c>
       <c r="D29">
         <f t="shared" si="1"/>
-        <v>3.7509999999999999</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2.7</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="2"/>
+        <v>34.370076037775853</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>691</v>
       </c>
@@ -18332,10 +19054,14 @@
       </c>
       <c r="D30">
         <f t="shared" si="1"/>
-        <v>3.851</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2.8</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="2"/>
+        <v>34.650754116555888</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>695</v>
       </c>
@@ -18348,10 +19074,14 @@
       </c>
       <c r="D31">
         <f t="shared" si="1"/>
-        <v>3.9510000000000001</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+        <v>2.9000000000000004</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="2"/>
+        <v>34.907041471334665</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>700</v>
       </c>
@@ -18364,10 +19094,14 @@
       </c>
       <c r="D32">
         <f t="shared" si="1"/>
-        <v>4.0510000000000002</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="2"/>
+        <v>35.141057638557257</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>704</v>
       </c>
@@ -18380,10 +19114,14 @@
       </c>
       <c r="D33">
         <f t="shared" si="1"/>
-        <v>4.1509999999999998</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3.0999999999999996</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="2"/>
+        <v>35.354737968469834</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>707</v>
       </c>
@@ -18396,10 +19134,14 @@
       </c>
       <c r="D34">
         <f t="shared" si="1"/>
-        <v>4.2510000000000003</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3.2</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="2"/>
+        <v>35.549849630768442</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>710</v>
       </c>
@@ -18412,10 +19154,14 @@
       </c>
       <c r="D35">
         <f t="shared" si="1"/>
-        <v>4.351</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3.3</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="2"/>
+        <v>35.728006229368319</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>714</v>
       </c>
@@ -18428,10 +19174,14 @@
       </c>
       <c r="D36">
         <f t="shared" si="1"/>
-        <v>4.4509999999999996</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3.3999999999999995</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="2"/>
+        <v>35.890681147160279</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>716</v>
       </c>
@@ -18444,10 +19194,14 @@
       </c>
       <c r="D37">
         <f t="shared" si="1"/>
-        <v>4.5510000000000002</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3.5</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="2"/>
+        <v>36.039219731117278</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>719</v>
       </c>
@@ -18460,10 +19214,14 @@
       </c>
       <c r="D38">
         <f t="shared" si="1"/>
-        <v>4.6509999999999998</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3.5999999999999996</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="2"/>
+        <v>36.17485041852396</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>722</v>
       </c>
@@ -18476,10 +19234,14 @@
       </c>
       <c r="D39">
         <f t="shared" si="1"/>
-        <v>4.7510000000000003</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3.7</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="2"/>
+        <v>36.298694896344863</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>723</v>
       </c>
@@ -18492,10 +19254,14 @@
       </c>
       <c r="D40">
         <f t="shared" si="1"/>
-        <v>4.851</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3.8</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="2"/>
+        <v>36.411777377750731</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>726</v>
       </c>
@@ -18508,10 +19274,14 @@
       </c>
       <c r="D41">
         <f t="shared" si="1"/>
-        <v>4.9509999999999996</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3.8999999999999995</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="2"/>
+        <v>36.515033072521405</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>728</v>
       </c>
@@ -18524,10 +19294,14 @@
       </c>
       <c r="D42">
         <f t="shared" si="1"/>
-        <v>5.0510000000000002</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="2"/>
+        <v>36.609315921376727</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>729</v>
       </c>
@@ -18540,10 +19314,14 @@
       </c>
       <c r="D43">
         <f t="shared" si="1"/>
-        <v>5.1509999999999998</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="2"/>
+        <v>36.695405658199661</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>731</v>
       </c>
@@ -18556,10 +19334,14 @@
       </c>
       <c r="D44">
         <f t="shared" si="1"/>
-        <v>5.2510000000000003</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4.2</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="2"/>
+        <v>36.774014258557223</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>733</v>
       </c>
@@ -18572,10 +19354,14 @@
       </c>
       <c r="D45">
         <f t="shared" si="1"/>
-        <v>5.351</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4.3</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="2"/>
+        <v>36.845791827849666</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>734</v>
       </c>
@@ -18588,10 +19374,14 @@
       </c>
       <c r="D46">
         <f t="shared" si="1"/>
-        <v>5.4509999999999996</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4.3999999999999995</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="2"/>
+        <v>36.911331977783597</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>735</v>
       </c>
@@ -18604,10 +19394,14 @@
       </c>
       <c r="D47">
         <f t="shared" si="1"/>
-        <v>5.5510000000000002</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4.5</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="2"/>
+        <v>36.971176735633513</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>737</v>
       </c>
@@ -18620,10 +19414,14 @@
       </c>
       <c r="D48">
         <f t="shared" si="1"/>
-        <v>5.6509999999999998</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="2"/>
+        <v>37.025821026892011</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>738</v>
       </c>
@@ -18636,10 +19434,14 @@
       </c>
       <c r="D49">
         <f t="shared" si="1"/>
-        <v>5.7510000000000003</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4.7</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="2"/>
+        <v>37.075716768380879</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>739</v>
       </c>
@@ -18652,10 +19454,14 @@
       </c>
       <c r="D50">
         <f t="shared" si="1"/>
-        <v>5.851</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4.8</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="2"/>
+        <v>37.121276605673806</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>740</v>
       </c>
@@ -18668,10 +19474,14 @@
       </c>
       <c r="D51">
         <f t="shared" si="1"/>
-        <v>5.9509999999999996</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4.8999999999999995</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="2"/>
+        <v>37.162877325739672</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>740</v>
       </c>
@@ -18684,10 +19494,14 @@
       </c>
       <c r="D52">
         <f t="shared" si="1"/>
-        <v>6.0510000000000002</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="2"/>
+        <v>37.200862973029679</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>742</v>
       </c>
@@ -18700,10 +19514,14 @@
       </c>
       <c r="D53">
         <f t="shared" si="1"/>
-        <v>6.1509999999999998</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="2"/>
+        <v>37.235547694778624</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>743</v>
       </c>
@@ -18716,10 +19534,14 @@
       </c>
       <c r="D54">
         <f t="shared" si="1"/>
-        <v>6.2510000000000003</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5.2</v>
+      </c>
+      <c r="E54">
+        <f t="shared" si="2"/>
+        <v>37.267218339051638</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>743</v>
       </c>
@@ -18732,10 +19554,14 @@
       </c>
       <c r="D55">
         <f t="shared" si="1"/>
-        <v>6.351</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5.3</v>
+      </c>
+      <c r="E55">
+        <f t="shared" si="2"/>
+        <v>37.296136827022451</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>744</v>
       </c>
@@ -18748,10 +19574,14 @@
       </c>
       <c r="D56">
         <f t="shared" si="1"/>
-        <v>6.4509999999999996</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5.3999999999999995</v>
+      </c>
+      <c r="E56">
+        <f t="shared" si="2"/>
+        <v>37.322542319102403</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>745</v>
       </c>
@@ -18764,10 +19594,14 @@
       </c>
       <c r="D57">
         <f t="shared" si="1"/>
-        <v>6.5510000000000002</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5.5</v>
+      </c>
+      <c r="E57">
+        <f t="shared" si="2"/>
+        <v>37.346653192834388</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>745</v>
       </c>
@@ -18780,10 +19614,14 @@
       </c>
       <c r="D58">
         <f t="shared" si="1"/>
-        <v>6.6509999999999998</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5.6</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="2"/>
+        <v>37.368668848909259</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>746</v>
       </c>
@@ -18796,10 +19634,14 @@
       </c>
       <c r="D59">
         <f t="shared" si="1"/>
-        <v>6.7510000000000003</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5.7</v>
+      </c>
+      <c r="E59">
+        <f t="shared" si="2"/>
+        <v>37.388771360240639</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>746</v>
       </c>
@@ -18812,10 +19654,14 @@
       </c>
       <c r="D60">
         <f t="shared" si="1"/>
-        <v>6.851</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5.8</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="2"/>
+        <v>37.407126977736404</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>747</v>
       </c>
@@ -18828,10 +19674,14 @@
       </c>
       <c r="D61">
         <f t="shared" si="1"/>
-        <v>6.9509999999999996</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5.8999999999999995</v>
+      </c>
+      <c r="E61">
+        <f t="shared" si="2"/>
+        <v>37.423887505219582</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>747</v>
       </c>
@@ -18844,10 +19694,14 @@
       </c>
       <c r="D62">
         <f t="shared" si="1"/>
-        <v>7.0510000000000002</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="E62">
+        <f t="shared" si="2"/>
+        <v>37.439191554869744</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>748</v>
       </c>
@@ -18860,10 +19714,14 @@
       </c>
       <c r="D63">
         <f t="shared" si="1"/>
-        <v>7.1509999999999998</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6.1</v>
+      </c>
+      <c r="E63">
+        <f t="shared" si="2"/>
+        <v>37.453165693567328</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>748</v>
       </c>
@@ -18876,10 +19734,14 @@
       </c>
       <c r="D64">
         <f t="shared" si="1"/>
-        <v>7.2510000000000003</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6.2</v>
+      </c>
+      <c r="E64">
+        <f t="shared" si="2"/>
+        <v>37.465925489621519</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>749</v>
       </c>
@@ -18892,10 +19754,14 @@
       </c>
       <c r="D65">
         <f t="shared" si="1"/>
-        <v>7.351</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6.3</v>
+      </c>
+      <c r="E65">
+        <f t="shared" si="2"/>
+        <v>37.477576468538217</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>748</v>
       </c>
@@ -18908,10 +19774,14 @@
       </c>
       <c r="D66">
         <f t="shared" si="1"/>
-        <v>7.4509999999999996</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+        <v>6.3999999999999995</v>
+      </c>
+      <c r="E66">
+        <f t="shared" si="2"/>
+        <v>37.488214985732441</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>749</v>
       </c>
@@ -18919,15 +19789,19 @@
         <v>7551</v>
       </c>
       <c r="C67">
-        <f t="shared" ref="C67:C130" si="2">A67/200/0.1</f>
+        <f t="shared" ref="C67:C130" si="3">A67/200/0.1</f>
         <v>37.449999999999996</v>
       </c>
       <c r="D67">
-        <f t="shared" ref="D67:D130" si="3">B67/1000</f>
-        <v>7.5510000000000002</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" ref="D67:D130" si="4">B67/1000 - 1.051</f>
+        <v>6.5</v>
+      </c>
+      <c r="E67">
+        <f t="shared" ref="E67:E92" si="5">$G$1*(1-EXP(-D67/$F$1))</f>
+        <v>37.497929023402669</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>750</v>
       </c>
@@ -18935,15 +19809,19 @@
         <v>7651</v>
       </c>
       <c r="C68">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>37.5</v>
       </c>
       <c r="D68">
-        <f t="shared" si="3"/>
-        <v>7.6509999999999998</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>6.6</v>
+      </c>
+      <c r="E68">
+        <f t="shared" si="5"/>
+        <v>37.506798918157344</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>749</v>
       </c>
@@ -18951,15 +19829,19 @@
         <v>7751</v>
       </c>
       <c r="C69">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>37.449999999999996</v>
       </c>
       <c r="D69">
-        <f t="shared" si="3"/>
-        <v>7.7510000000000003</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>6.7</v>
+      </c>
+      <c r="E69">
+        <f t="shared" si="5"/>
+        <v>37.514898025411192</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>750</v>
       </c>
@@ -18967,15 +19849,19 @@
         <v>7851</v>
       </c>
       <c r="C70">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>37.5</v>
       </c>
       <c r="D70">
-        <f t="shared" si="3"/>
-        <v>7.851</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>6.8</v>
+      </c>
+      <c r="E70">
+        <f t="shared" si="5"/>
+        <v>37.522293326045926</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>750</v>
       </c>
@@ -18983,15 +19869,19 @@
         <v>7951</v>
       </c>
       <c r="C71">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>37.5</v>
       </c>
       <c r="D71">
-        <f t="shared" si="3"/>
-        <v>7.9509999999999996</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>6.8999999999999995</v>
+      </c>
+      <c r="E71">
+        <f t="shared" si="5"/>
+        <v>37.52904598035262</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>750</v>
       </c>
@@ -18999,15 +19889,19 @@
         <v>8051</v>
       </c>
       <c r="C72">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>37.5</v>
       </c>
       <c r="D72">
-        <f t="shared" si="3"/>
-        <v>8.0510000000000002</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="E72">
+        <f t="shared" si="5"/>
+        <v>37.535211833836868</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>751</v>
       </c>
@@ -19015,15 +19909,19 @@
         <v>8151</v>
       </c>
       <c r="C73">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>37.549999999999997</v>
       </c>
       <c r="D73">
-        <f t="shared" si="3"/>
-        <v>8.1509999999999998</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>7.1</v>
+      </c>
+      <c r="E73">
+        <f t="shared" si="5"/>
+        <v>37.540841879069831</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>750</v>
       </c>
@@ -19031,15 +19929,19 @@
         <v>8251</v>
       </c>
       <c r="C74">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>37.5</v>
       </c>
       <c r="D74">
-        <f t="shared" si="3"/>
-        <v>8.2509999999999994</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>7.1999999999999993</v>
+      </c>
+      <c r="E74">
+        <f t="shared" si="5"/>
+        <v>37.545982677404751</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>751</v>
       </c>
@@ -19047,15 +19949,19 @@
         <v>8351</v>
       </c>
       <c r="C75">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>37.549999999999997</v>
       </c>
       <c r="D75">
-        <f t="shared" si="3"/>
-        <v>8.3510000000000009</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>7.3000000000000007</v>
+      </c>
+      <c r="E75">
+        <f t="shared" si="5"/>
+        <v>37.550676744046633</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>751</v>
       </c>
@@ -19063,15 +19969,19 @@
         <v>8451</v>
       </c>
       <c r="C76">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>37.549999999999997</v>
       </c>
       <c r="D76">
-        <f t="shared" si="3"/>
-        <v>8.4510000000000005</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>7.4</v>
+      </c>
+      <c r="E76">
+        <f t="shared" si="5"/>
+        <v>37.554962899659607</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>751</v>
       </c>
@@ -19079,15 +19989,19 @@
         <v>8551</v>
       </c>
       <c r="C77">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>37.549999999999997</v>
       </c>
       <c r="D77">
-        <f t="shared" si="3"/>
-        <v>8.5510000000000002</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>7.5</v>
+      </c>
+      <c r="E77">
+        <f t="shared" si="5"/>
+        <v>37.55887659141991</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>751</v>
       </c>
@@ -19095,15 +20009,19 @@
         <v>8651</v>
       </c>
       <c r="C78">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>37.549999999999997</v>
       </c>
       <c r="D78">
-        <f t="shared" si="3"/>
-        <v>8.6509999999999998</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>7.6</v>
+      </c>
+      <c r="E78">
+        <f t="shared" si="5"/>
+        <v>37.562450186169556</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>751</v>
       </c>
@@ -19111,15 +20029,19 @@
         <v>8751</v>
       </c>
       <c r="C79">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>37.549999999999997</v>
       </c>
       <c r="D79">
-        <f t="shared" si="3"/>
-        <v>8.7509999999999994</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>7.6999999999999993</v>
+      </c>
+      <c r="E79">
+        <f t="shared" si="5"/>
+        <v>37.565713238095157</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>751</v>
       </c>
@@ -19127,15 +20049,19 @@
         <v>8851</v>
       </c>
       <c r="C80">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>37.549999999999997</v>
       </c>
       <c r="D80">
-        <f t="shared" si="3"/>
-        <v>8.8510000000000009</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>7.8000000000000007</v>
+      </c>
+      <c r="E80">
+        <f t="shared" si="5"/>
+        <v>37.568692733145689</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>752</v>
       </c>
@@ -19143,15 +20069,19 @@
         <v>8951</v>
       </c>
       <c r="C81">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>37.599999999999994</v>
       </c>
       <c r="D81">
-        <f t="shared" si="3"/>
-        <v>8.9510000000000005</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>7.9</v>
+      </c>
+      <c r="E81">
+        <f t="shared" si="5"/>
+        <v>37.571413312210481</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>752</v>
       </c>
@@ -19159,15 +20089,19 @@
         <v>9051</v>
       </c>
       <c r="C82">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>37.599999999999994</v>
       </c>
       <c r="D82">
-        <f t="shared" si="3"/>
-        <v>9.0510000000000002</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="E82">
+        <f t="shared" si="5"/>
+        <v>37.573897474903255</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>751</v>
       </c>
@@ -19175,15 +20109,19 @@
         <v>9151</v>
       </c>
       <c r="C83">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>37.549999999999997</v>
       </c>
       <c r="D83">
-        <f t="shared" si="3"/>
-        <v>9.1509999999999998</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>8.1</v>
+      </c>
+      <c r="E83">
+        <f t="shared" si="5"/>
+        <v>37.576165765637384</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>752</v>
       </c>
@@ -19191,15 +20129,19 @@
         <v>9251</v>
       </c>
       <c r="C84">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>37.599999999999994</v>
       </c>
       <c r="D84">
-        <f t="shared" si="3"/>
-        <v>9.2509999999999994</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="E84">
+        <f t="shared" si="5"/>
+        <v>37.578236943531458</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>751</v>
       </c>
@@ -19207,15 +20149,19 @@
         <v>9351</v>
       </c>
       <c r="C85">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>37.549999999999997</v>
       </c>
       <c r="D85">
-        <f t="shared" si="3"/>
-        <v>9.3510000000000009</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="E85">
+        <f t="shared" si="5"/>
+        <v>37.580128137550084</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>752</v>
       </c>
@@ -19223,15 +20169,19 @@
         <v>9451</v>
       </c>
       <c r="C86">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>37.599999999999994</v>
       </c>
       <c r="D86">
-        <f t="shared" si="3"/>
-        <v>9.4510000000000005</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>8.4</v>
+      </c>
+      <c r="E86">
+        <f t="shared" si="5"/>
+        <v>37.581854988163123</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>752</v>
       </c>
@@ -19239,15 +20189,19 @@
         <v>9551</v>
       </c>
       <c r="C87">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>37.599999999999994</v>
       </c>
       <c r="D87">
-        <f t="shared" si="3"/>
-        <v>9.5510000000000002</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>8.5</v>
+      </c>
+      <c r="E87">
+        <f t="shared" si="5"/>
+        <v>37.583431776694795</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>752</v>
       </c>
@@ -19255,15 +20209,19 @@
         <v>9651</v>
       </c>
       <c r="C88">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>37.599999999999994</v>
       </c>
       <c r="D88">
-        <f t="shared" si="3"/>
-        <v>9.6509999999999998</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>8.6</v>
+      </c>
+      <c r="E88">
+        <f t="shared" si="5"/>
+        <v>37.584871543432492</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>752</v>
       </c>
@@ -19271,15 +20229,19 @@
         <v>9751</v>
       </c>
       <c r="C89">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>37.599999999999994</v>
       </c>
       <c r="D89">
-        <f t="shared" si="3"/>
-        <v>9.7509999999999994</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="E89">
+        <f t="shared" si="5"/>
+        <v>37.586186195471967</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>752</v>
       </c>
@@ -19287,15 +20249,19 @@
         <v>9851</v>
       </c>
       <c r="C90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>37.599999999999994</v>
       </c>
       <c r="D90">
-        <f t="shared" si="3"/>
-        <v>9.8510000000000009</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="E90">
+        <f t="shared" si="5"/>
+        <v>37.587386605190865</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>752</v>
       </c>
@@ -19303,15 +20269,19 @@
         <v>9951</v>
       </c>
       <c r="C91">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>37.599999999999994</v>
       </c>
       <c r="D91">
-        <f t="shared" si="3"/>
-        <v>9.9510000000000005</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>8.9</v>
+      </c>
+      <c r="E91">
+        <f t="shared" si="5"/>
+        <v>37.588482700165031</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>752</v>
       </c>
@@ -19319,15 +20289,19 @@
         <v>10051</v>
       </c>
       <c r="C92">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>37.599999999999994</v>
       </c>
       <c r="D92">
-        <f t="shared" si="3"/>
-        <v>10.051</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="E92">
+        <f t="shared" si="5"/>
+        <v>37.589483545271051</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>735</v>
       </c>
@@ -19335,15 +20309,15 @@
         <v>10151</v>
       </c>
       <c r="C93">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>36.749999999999993</v>
       </c>
       <c r="D93">
-        <f t="shared" si="3"/>
-        <v>10.151</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>9.1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>701</v>
       </c>
@@ -19351,15 +20325,15 @@
         <v>10251</v>
       </c>
       <c r="C94">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>35.049999999999997</v>
       </c>
       <c r="D94">
-        <f t="shared" si="3"/>
-        <v>10.250999999999999</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>9.1999999999999993</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>666</v>
       </c>
@@ -19367,15 +20341,15 @@
         <v>10351</v>
       </c>
       <c r="C95">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>33.299999999999997</v>
       </c>
       <c r="D95">
-        <f t="shared" si="3"/>
-        <v>10.351000000000001</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>9.3000000000000007</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>631</v>
       </c>
@@ -19383,12 +20357,12 @@
         <v>10451</v>
       </c>
       <c r="C96">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>31.549999999999997</v>
       </c>
       <c r="D96">
-        <f t="shared" si="3"/>
-        <v>10.451000000000001</v>
+        <f t="shared" si="4"/>
+        <v>9.4</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -19399,12 +20373,12 @@
         <v>10551</v>
       </c>
       <c r="C97">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>29.75</v>
       </c>
       <c r="D97">
-        <f t="shared" si="3"/>
-        <v>10.551</v>
+        <f t="shared" si="4"/>
+        <v>9.5</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -19415,12 +20389,12 @@
         <v>10651</v>
       </c>
       <c r="C98">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>27.85</v>
       </c>
       <c r="D98">
-        <f t="shared" si="3"/>
-        <v>10.651</v>
+        <f t="shared" si="4"/>
+        <v>9.6</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -19431,12 +20405,12 @@
         <v>10751</v>
       </c>
       <c r="C99">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>26</v>
       </c>
       <c r="D99">
-        <f t="shared" si="3"/>
-        <v>10.750999999999999</v>
+        <f t="shared" si="4"/>
+        <v>9.6999999999999993</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -19447,12 +20421,12 @@
         <v>10851</v>
       </c>
       <c r="C100">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>24.1</v>
       </c>
       <c r="D100">
-        <f t="shared" si="3"/>
-        <v>10.851000000000001</v>
+        <f t="shared" si="4"/>
+        <v>9.8000000000000007</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -19463,12 +20437,12 @@
         <v>10951</v>
       </c>
       <c r="C101">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>22.15</v>
       </c>
       <c r="D101">
-        <f t="shared" si="3"/>
-        <v>10.951000000000001</v>
+        <f t="shared" si="4"/>
+        <v>9.9</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -19479,12 +20453,12 @@
         <v>11051</v>
       </c>
       <c r="C102">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>20.149999999999999</v>
       </c>
       <c r="D102">
-        <f t="shared" si="3"/>
-        <v>11.051</v>
+        <f t="shared" si="4"/>
+        <v>10</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -19495,12 +20469,12 @@
         <v>11151</v>
       </c>
       <c r="C103">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>18.25</v>
       </c>
       <c r="D103">
-        <f t="shared" si="3"/>
-        <v>11.151</v>
+        <f t="shared" si="4"/>
+        <v>10.1</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -19511,12 +20485,12 @@
         <v>11251</v>
       </c>
       <c r="C104">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>16.25</v>
       </c>
       <c r="D104">
-        <f t="shared" si="3"/>
-        <v>11.250999999999999</v>
+        <f t="shared" si="4"/>
+        <v>10.199999999999999</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -19527,12 +20501,12 @@
         <v>11351</v>
       </c>
       <c r="C105">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>14.399999999999999</v>
       </c>
       <c r="D105">
-        <f t="shared" si="3"/>
-        <v>11.351000000000001</v>
+        <f t="shared" si="4"/>
+        <v>10.3</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -19543,12 +20517,12 @@
         <v>11451</v>
       </c>
       <c r="C106">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>12.549999999999999</v>
       </c>
       <c r="D106">
-        <f t="shared" si="3"/>
-        <v>11.451000000000001</v>
+        <f t="shared" si="4"/>
+        <v>10.4</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -19559,12 +20533,12 @@
         <v>11551</v>
       </c>
       <c r="C107">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>10.8</v>
       </c>
       <c r="D107">
-        <f t="shared" si="3"/>
-        <v>11.551</v>
+        <f t="shared" si="4"/>
+        <v>10.5</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -19575,12 +20549,12 @@
         <v>11651</v>
       </c>
       <c r="C108">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9.25</v>
       </c>
       <c r="D108">
-        <f t="shared" si="3"/>
-        <v>11.651</v>
+        <f t="shared" si="4"/>
+        <v>10.6</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -19591,12 +20565,12 @@
         <v>11751</v>
       </c>
       <c r="C109">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.75</v>
       </c>
       <c r="D109">
-        <f t="shared" si="3"/>
-        <v>11.750999999999999</v>
+        <f t="shared" si="4"/>
+        <v>10.7</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -19607,12 +20581,12 @@
         <v>11851</v>
       </c>
       <c r="C110">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6.5</v>
       </c>
       <c r="D110">
-        <f t="shared" si="3"/>
-        <v>11.851000000000001</v>
+        <f t="shared" si="4"/>
+        <v>10.8</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -19623,12 +20597,12 @@
         <v>11951</v>
       </c>
       <c r="C111">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.4</v>
       </c>
       <c r="D111">
-        <f t="shared" si="3"/>
-        <v>11.951000000000001</v>
+        <f t="shared" si="4"/>
+        <v>10.9</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
@@ -19639,12 +20613,12 @@
         <v>12051</v>
       </c>
       <c r="C112">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4.3999999999999995</v>
       </c>
       <c r="D112">
-        <f t="shared" si="3"/>
-        <v>12.051</v>
+        <f t="shared" si="4"/>
+        <v>11</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
@@ -19655,12 +20629,12 @@
         <v>12151</v>
       </c>
       <c r="C113">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.5999999999999996</v>
       </c>
       <c r="D113">
-        <f t="shared" si="3"/>
-        <v>12.151</v>
+        <f t="shared" si="4"/>
+        <v>11.1</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
@@ -19671,12 +20645,12 @@
         <v>12251</v>
       </c>
       <c r="C114">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.9499999999999997</v>
       </c>
       <c r="D114">
-        <f t="shared" si="3"/>
-        <v>12.250999999999999</v>
+        <f t="shared" si="4"/>
+        <v>11.2</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
@@ -19687,12 +20661,12 @@
         <v>12351</v>
       </c>
       <c r="C115">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.3499999999999996</v>
       </c>
       <c r="D115">
-        <f t="shared" si="3"/>
-        <v>12.351000000000001</v>
+        <f t="shared" si="4"/>
+        <v>11.3</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -19703,12 +20677,12 @@
         <v>12451</v>
       </c>
       <c r="C116">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.8499999999999999</v>
       </c>
       <c r="D116">
-        <f t="shared" si="3"/>
-        <v>12.451000000000001</v>
+        <f t="shared" si="4"/>
+        <v>11.4</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
@@ -19719,12 +20693,12 @@
         <v>12551</v>
       </c>
       <c r="C117">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.4999999999999998</v>
       </c>
       <c r="D117">
-        <f t="shared" si="3"/>
-        <v>12.551</v>
+        <f t="shared" si="4"/>
+        <v>11.5</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
@@ -19735,12 +20709,12 @@
         <v>12651</v>
       </c>
       <c r="C118">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.1499999999999999</v>
       </c>
       <c r="D118">
-        <f t="shared" si="3"/>
-        <v>12.651</v>
+        <f t="shared" si="4"/>
+        <v>11.6</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -19751,12 +20725,12 @@
         <v>12751</v>
       </c>
       <c r="C119">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.89999999999999991</v>
       </c>
       <c r="D119">
-        <f t="shared" si="3"/>
-        <v>12.750999999999999</v>
+        <f t="shared" si="4"/>
+        <v>11.7</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -19767,12 +20741,12 @@
         <v>12851</v>
       </c>
       <c r="C120">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.70000000000000007</v>
       </c>
       <c r="D120">
-        <f t="shared" si="3"/>
-        <v>12.851000000000001</v>
+        <f t="shared" si="4"/>
+        <v>11.8</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
@@ -19783,12 +20757,12 @@
         <v>12951</v>
       </c>
       <c r="C121">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.44999999999999996</v>
       </c>
       <c r="D121">
-        <f t="shared" si="3"/>
-        <v>12.951000000000001</v>
+        <f t="shared" si="4"/>
+        <v>11.9</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -19799,12 +20773,12 @@
         <v>13051</v>
       </c>
       <c r="C122">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.35000000000000003</v>
       </c>
       <c r="D122">
-        <f t="shared" si="3"/>
-        <v>13.051</v>
+        <f t="shared" si="4"/>
+        <v>12</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
@@ -19815,12 +20789,12 @@
         <v>13151</v>
       </c>
       <c r="C123">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.25</v>
       </c>
       <c r="D123">
-        <f t="shared" si="3"/>
-        <v>13.151</v>
+        <f t="shared" si="4"/>
+        <v>12.1</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -19831,12 +20805,12 @@
         <v>13251</v>
       </c>
       <c r="C124">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9.9999999999999992E-2</v>
       </c>
       <c r="D124">
-        <f t="shared" si="3"/>
-        <v>13.250999999999999</v>
+        <f t="shared" si="4"/>
+        <v>12.2</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -19847,12 +20821,12 @@
         <v>13351</v>
       </c>
       <c r="C125">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4.9999999999999996E-2</v>
       </c>
       <c r="D125">
-        <f t="shared" si="3"/>
-        <v>13.351000000000001</v>
+        <f t="shared" si="4"/>
+        <v>12.3</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -19863,12 +20837,12 @@
         <v>13451</v>
       </c>
       <c r="C126">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-4.9999999999999996E-2</v>
       </c>
       <c r="D126">
-        <f t="shared" si="3"/>
-        <v>13.451000000000001</v>
+        <f t="shared" si="4"/>
+        <v>12.4</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
@@ -19879,12 +20853,12 @@
         <v>13551</v>
       </c>
       <c r="C127">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="D127">
-        <f t="shared" si="3"/>
-        <v>13.551</v>
+        <f t="shared" si="4"/>
+        <v>12.5</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
@@ -19895,12 +20869,12 @@
         <v>13651</v>
       </c>
       <c r="C128">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="D128">
-        <f t="shared" si="3"/>
-        <v>13.651</v>
+        <f t="shared" si="4"/>
+        <v>12.6</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
@@ -19911,12 +20885,12 @@
         <v>13751</v>
       </c>
       <c r="C129">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="D129">
-        <f t="shared" si="3"/>
-        <v>13.750999999999999</v>
+        <f t="shared" si="4"/>
+        <v>12.7</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
@@ -19927,12 +20901,12 @@
         <v>13851</v>
       </c>
       <c r="C130">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="D130">
-        <f t="shared" si="3"/>
-        <v>13.851000000000001</v>
+        <f t="shared" si="4"/>
+        <v>12.8</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
@@ -19943,12 +20917,12 @@
         <v>13951</v>
       </c>
       <c r="C131">
-        <f t="shared" ref="C131:C194" si="4">A131/200/0.1</f>
+        <f t="shared" ref="C131:C150" si="6">A131/200/0.1</f>
         <v>0</v>
       </c>
       <c r="D131">
-        <f t="shared" ref="D131:D194" si="5">B131/1000</f>
-        <v>13.951000000000001</v>
+        <f t="shared" ref="D131:D150" si="7">B131/1000 - 1.051</f>
+        <v>12.9</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -19959,12 +20933,12 @@
         <v>14051</v>
       </c>
       <c r="C132">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D132">
-        <f t="shared" si="5"/>
-        <v>14.051</v>
+        <f t="shared" si="7"/>
+        <v>13</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
@@ -19975,12 +20949,12 @@
         <v>14151</v>
       </c>
       <c r="C133">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D133">
-        <f t="shared" si="5"/>
-        <v>14.151</v>
+        <f t="shared" si="7"/>
+        <v>13.1</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
@@ -19991,12 +20965,12 @@
         <v>14251</v>
       </c>
       <c r="C134">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D134">
-        <f t="shared" si="5"/>
-        <v>14.250999999999999</v>
+        <f t="shared" si="7"/>
+        <v>13.2</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
@@ -20007,12 +20981,12 @@
         <v>14351</v>
       </c>
       <c r="C135">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D135">
-        <f t="shared" si="5"/>
-        <v>14.351000000000001</v>
+        <f t="shared" si="7"/>
+        <v>13.3</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
@@ -20023,12 +20997,12 @@
         <v>14451</v>
       </c>
       <c r="C136">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D136">
-        <f t="shared" si="5"/>
-        <v>14.451000000000001</v>
+        <f t="shared" si="7"/>
+        <v>13.4</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
@@ -20039,12 +21013,12 @@
         <v>14551</v>
       </c>
       <c r="C137">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D137">
-        <f t="shared" si="5"/>
-        <v>14.551</v>
+        <f t="shared" si="7"/>
+        <v>13.5</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
@@ -20055,12 +21029,12 @@
         <v>14651</v>
       </c>
       <c r="C138">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D138">
-        <f t="shared" si="5"/>
-        <v>14.651</v>
+        <f t="shared" si="7"/>
+        <v>13.6</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
@@ -20071,12 +21045,12 @@
         <v>14751</v>
       </c>
       <c r="C139">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D139">
-        <f t="shared" si="5"/>
-        <v>14.750999999999999</v>
+        <f t="shared" si="7"/>
+        <v>13.7</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
@@ -20087,12 +21061,12 @@
         <v>14851</v>
       </c>
       <c r="C140">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D140">
-        <f t="shared" si="5"/>
-        <v>14.851000000000001</v>
+        <f t="shared" si="7"/>
+        <v>13.8</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
@@ -20103,12 +21077,12 @@
         <v>14951</v>
       </c>
       <c r="C141">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D141">
-        <f t="shared" si="5"/>
-        <v>14.951000000000001</v>
+        <f t="shared" si="7"/>
+        <v>13.9</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
@@ -20119,12 +21093,12 @@
         <v>15051</v>
       </c>
       <c r="C142">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D142">
-        <f t="shared" si="5"/>
-        <v>15.051</v>
+        <f t="shared" si="7"/>
+        <v>14</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
@@ -20135,12 +21109,12 @@
         <v>15151</v>
       </c>
       <c r="C143">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D143">
-        <f t="shared" si="5"/>
-        <v>15.151</v>
+        <f t="shared" si="7"/>
+        <v>14.1</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
@@ -20151,12 +21125,12 @@
         <v>15251</v>
       </c>
       <c r="C144">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D144">
-        <f t="shared" si="5"/>
-        <v>15.250999999999999</v>
+        <f t="shared" si="7"/>
+        <v>14.2</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
@@ -20167,12 +21141,12 @@
         <v>15351</v>
       </c>
       <c r="C145">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D145">
-        <f t="shared" si="5"/>
-        <v>15.351000000000001</v>
+        <f t="shared" si="7"/>
+        <v>14.3</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
@@ -20183,12 +21157,12 @@
         <v>15451</v>
       </c>
       <c r="C146">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D146">
-        <f t="shared" si="5"/>
-        <v>15.451000000000001</v>
+        <f t="shared" si="7"/>
+        <v>14.4</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
@@ -20199,12 +21173,12 @@
         <v>15551</v>
       </c>
       <c r="C147">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D147">
-        <f t="shared" si="5"/>
-        <v>15.551</v>
+        <f t="shared" si="7"/>
+        <v>14.5</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
@@ -20215,12 +21189,12 @@
         <v>15651</v>
       </c>
       <c r="C148">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D148">
-        <f t="shared" si="5"/>
-        <v>15.651</v>
+        <f t="shared" si="7"/>
+        <v>14.6</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
@@ -20231,12 +21205,12 @@
         <v>15751</v>
       </c>
       <c r="C149">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D149">
-        <f t="shared" si="5"/>
-        <v>15.750999999999999</v>
+        <f t="shared" si="7"/>
+        <v>14.7</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
@@ -20247,12 +21221,12 @@
         <v>15851</v>
       </c>
       <c r="C150">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="D150">
-        <f t="shared" si="5"/>
-        <v>15.851000000000001</v>
+        <f t="shared" si="7"/>
+        <v>14.8</v>
       </c>
     </row>
   </sheetData>
@@ -20265,7 +21239,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F934D63D-5EA6-49FC-924F-91CDEED72800}">
   <dimension ref="A1:D184"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A141" workbookViewId="0">
+    <sheetView topLeftCell="A141" workbookViewId="0">
       <selection activeCell="X164" sqref="X164"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
stable code with long term balance
</commit_message>
<xml_diff>
--- a/MotorData.xlsx
+++ b/MotorData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark\Documents\GitHub\Cube\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E475622F-A623-40B2-A507-490DFFFA9955}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D72A773-6C21-47CB-972A-C66ED4F3B029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{EC7B1352-56D2-4F86-A349-4A1459A01683}"/>
+    <workbookView minimized="1" xWindow="6600" yWindow="1965" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{EC7B1352-56D2-4F86-A349-4A1459A01683}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4643,274 +4643,274 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.2674130677869373</c:v>
+                  <c:v>3.3391243888651196</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.25089028037321</c:v>
+                  <c:v>6.3817128286793281</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.9751054601975486</c:v>
+                  <c:v>9.1540996391142233</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11.46258829220216</c:v>
+                  <c:v>11.680280481089243</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13.733910647845402</c:v>
+                  <c:v>13.982120044869507</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>15.807856717691163</c:v>
+                  <c:v>16.079541294110591</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>17.701578359598106</c:v>
+                  <c:v>17.990697903802079</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>19.430736947262563</c:v>
+                  <c:v>19.732131384600969</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>21.009632892224605</c:v>
+                  <c:v>21.318914253503007</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>22.451323910504602</c:v>
+                  <c:v>22.764780490027803</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>23.767733011953769</c:v>
+                  <c:v>24.082244407046836</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>24.969747105407496</c:v>
+                  <c:v>25.282708965109276</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>26.067307035121466</c:v>
+                  <c:v>26.376564467751649</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>27.069489793106001</c:v>
+                  <c:v>27.37327849202255</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>27.984583587267416</c:v>
+                  <c:v>28.281477832592198</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>28.820156386181658</c:v>
+                  <c:v>29.109023168692506</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>29.583118507376224</c:v>
+                  <c:v>29.863077100147493</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>30.279779766735217</c:v>
+                  <c:v>30.550166141362034</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>30.915901661662019</c:v>
+                  <c:v>31.176237209841421</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>31.49674501956251</c:v>
+                  <c:v>31.746709098163304</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>32.027113505709238</c:v>
+                  <c:v>32.266519374903865</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>32.511393350303365</c:v>
+                  <c:v>32.740167120457009</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>32.953589623283314</c:v>
+                  <c:v>33.171751867634946</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>33.357359356878661</c:v>
+                  <c:v>33.565009084090441</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>33.726041789837666</c:v>
+                  <c:v>33.92334250366924</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>34.062685983453221</c:v>
+                  <c:v>34.249853586528324</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>34.370076037775853</c:v>
+                  <c:v>34.547368363004189</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>34.650754116555888</c:v>
+                  <c:v>34.818461893571047</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>34.907041471334665</c:v>
+                  <c:v>35.065480556595908</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>35.141057638557257</c:v>
+                  <c:v>35.290562356795995</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>35.354737968469834</c:v>
+                  <c:v>35.495655430173279</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>35.549849630768442</c:v>
+                  <c:v>35.682534905590408</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>35.728006229368319</c:v>
+                  <c:v>35.852818268929255</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>35.890681147160279</c:v>
+                  <c:v>36.007979362812179</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>36.039219731117278</c:v>
+                  <c:v>36.149361143057142</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>36.17485041852396</c:v>
+                  <c:v>36.278187302276642</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>36.298694896344863</c:v>
+                  <c:v>36.395572861225567</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>36.411777377750731</c:v>
+                  <c:v>36.502533819568463</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>36.515033072521405</c:v>
+                  <c:v>36.59999594959595</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>36.609315921376727</c:v>
+                  <c:v>36.688802809002013</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>36.695405658199661</c:v>
+                  <c:v>36.769723042074538</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>36.774014258557223</c:v>
+                  <c:v>36.843457032492665</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>36.845791827849666</c:v>
+                  <c:v>36.910642965312562</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>36.911331977783597</c:v>
+                  <c:v>36.971862350609385</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>36.971176735633513</c:v>
+                  <c:v>37.027645056583978</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>37.025821026892011</c:v>
+                  <c:v>37.078473895696952</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>37.075716768380879</c:v>
+                  <c:v>37.124788803524297</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>37.121276605673806</c:v>
+                  <c:v>37.166990646503386</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>37.162877325739672</c:v>
+                  <c:v>37.205444691526452</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>37.200862973029679</c:v>
+                  <c:v>37.240483767411568</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>37.235547694778624</c:v>
+                  <c:v>37.272411145614463</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>37.267218339051638</c:v>
+                  <c:v>37.30150316511444</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>37.296136827022451</c:v>
+                  <c:v>37.328011624193309</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>37.322542319102403</c:v>
+                  <c:v>37.352165959808836</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>37.346653192834388</c:v>
+                  <c:v>37.374175233425682</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>37.368668848909259</c:v>
+                  <c:v>37.394229940491584</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>37.388771360240639</c:v>
+                  <c:v>37.412503659220384</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>37.407126977736404</c:v>
+                  <c:v>37.429154552952305</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>37.423887505219582</c:v>
+                  <c:v>37.444326739094954</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>37.439191554869744</c:v>
+                  <c:v>37.458151536493411</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>37.453165693567328</c:v>
+                  <c:v>37.470748602025807</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>37.465925489621519</c:v>
+                  <c:v>37.482226966261727</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>37.477576468538217</c:v>
+                  <c:v>37.492685977147524</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>37.488214985732441</c:v>
+                  <c:v>37.502216159886196</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>37.497929023402669</c:v>
+                  <c:v>37.510900000454299</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>37.506798918157344</c:v>
+                  <c:v>37.518812659537573</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>37.514898025411192</c:v>
+                  <c:v>37.526022623064307</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>37.522293326045926</c:v>
+                  <c:v>37.532592294967237</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>37.52904598035262</c:v>
+                  <c:v>37.538578537304268</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>37.535211833836868</c:v>
+                  <c:v>37.544033162412966</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>37.540841879069831</c:v>
+                  <c:v>37.549003381358567</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>37.545982677404751</c:v>
+                  <c:v>37.553532212556846</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>37.550676744046633</c:v>
+                  <c:v>37.557658854108652</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>37.554962899659607</c:v>
+                  <c:v>37.561419023068716</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>37.55887659141991</c:v>
+                  <c:v>37.564845264585138</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>37.562450186169556</c:v>
+                  <c:v>37.56796723358535</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>37.565713238095157</c:v>
+                  <c:v>37.570811951446466</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>37.568692733145689</c:v>
+                  <c:v>37.57340403987169</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>37.571413312210481</c:v>
+                  <c:v>37.575765933996948</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>37.573897474903255</c:v>
+                  <c:v>37.577918076572274</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>37.576165765637384</c:v>
+                  <c:v>37.579879094898615</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>37.578236943531458</c:v>
+                  <c:v>37.581665962051545</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>37.580128137550084</c:v>
+                  <c:v>37.583294143787185</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>37.581854988163123</c:v>
+                  <c:v>37.584777732402003</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>37.583431776694795</c:v>
+                  <c:v>37.586129568704933</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>37.584871543432492</c:v>
+                  <c:v>37.587361353157632</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>37.586186195471967</c:v>
+                  <c:v>37.5884837471447</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>37.587386605190865</c:v>
+                  <c:v>37.58950646525048</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>37.588482700165031</c:v>
+                  <c:v>37.590438359341107</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>37.589483545271051</c:v>
+                  <c:v>37.591287495179451</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -18474,8 +18474,7 @@
         <v>2</v>
       </c>
       <c r="F1">
-        <f>1.1</f>
-        <v>1.1000000000000001</v>
+        <v>0.93</v>
       </c>
       <c r="G1">
         <v>37.6</v>
@@ -18497,7 +18496,7 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <f>$G$1*(1-EXP(-D2/$F$1))</f>
+        <f>$G$1*(1-EXP(-D2*$F$1))</f>
         <v>0</v>
       </c>
     </row>
@@ -18517,8 +18516,8 @@
         <v>0.10000000000000009</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E66" si="2">$G$1*(1-EXP(-D3/$F$1))</f>
-        <v>3.2674130677869373</v>
+        <f t="shared" ref="E3:E66" si="2">$G$1*(1-EXP(-D3*$F$1))</f>
+        <v>3.3391243888651196</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -18538,7 +18537,7 @@
       </c>
       <c r="E4">
         <f t="shared" si="2"/>
-        <v>6.25089028037321</v>
+        <v>6.3817128286793281</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -18558,7 +18557,7 @@
       </c>
       <c r="E5">
         <f t="shared" si="2"/>
-        <v>8.9751054601975486</v>
+        <v>9.1540996391142233</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -18578,7 +18577,7 @@
       </c>
       <c r="E6">
         <f t="shared" si="2"/>
-        <v>11.46258829220216</v>
+        <v>11.680280481089243</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -18598,7 +18597,7 @@
       </c>
       <c r="E7">
         <f t="shared" si="2"/>
-        <v>13.733910647845402</v>
+        <v>13.982120044869507</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -18618,7 +18617,7 @@
       </c>
       <c r="E8">
         <f t="shared" si="2"/>
-        <v>15.807856717691163</v>
+        <v>16.079541294110591</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -18638,7 +18637,7 @@
       </c>
       <c r="E9">
         <f t="shared" si="2"/>
-        <v>17.701578359598106</v>
+        <v>17.990697903802079</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -18658,7 +18657,7 @@
       </c>
       <c r="E10">
         <f t="shared" si="2"/>
-        <v>19.430736947262563</v>
+        <v>19.732131384600969</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -18678,7 +18677,7 @@
       </c>
       <c r="E11">
         <f t="shared" si="2"/>
-        <v>21.009632892224605</v>
+        <v>21.318914253503007</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -18698,7 +18697,7 @@
       </c>
       <c r="E12">
         <f t="shared" si="2"/>
-        <v>22.451323910504602</v>
+        <v>22.764780490027803</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -18718,7 +18717,7 @@
       </c>
       <c r="E13">
         <f t="shared" si="2"/>
-        <v>23.767733011953769</v>
+        <v>24.082244407046836</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -18738,7 +18737,7 @@
       </c>
       <c r="E14">
         <f t="shared" si="2"/>
-        <v>24.969747105407496</v>
+        <v>25.282708965109276</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -18758,7 +18757,7 @@
       </c>
       <c r="E15">
         <f t="shared" si="2"/>
-        <v>26.067307035121466</v>
+        <v>26.376564467751649</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -18778,7 +18777,7 @@
       </c>
       <c r="E16">
         <f t="shared" si="2"/>
-        <v>27.069489793106001</v>
+        <v>27.37327849202255</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -18798,7 +18797,7 @@
       </c>
       <c r="E17">
         <f t="shared" si="2"/>
-        <v>27.984583587267416</v>
+        <v>28.281477832592198</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -18818,7 +18817,7 @@
       </c>
       <c r="E18">
         <f t="shared" si="2"/>
-        <v>28.820156386181658</v>
+        <v>29.109023168692506</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -18838,7 +18837,7 @@
       </c>
       <c r="E19">
         <f t="shared" si="2"/>
-        <v>29.583118507376224</v>
+        <v>29.863077100147493</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -18858,7 +18857,7 @@
       </c>
       <c r="E20">
         <f t="shared" si="2"/>
-        <v>30.279779766735217</v>
+        <v>30.550166141362034</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -18878,7 +18877,7 @@
       </c>
       <c r="E21">
         <f t="shared" si="2"/>
-        <v>30.915901661662019</v>
+        <v>31.176237209841421</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -18898,7 +18897,7 @@
       </c>
       <c r="E22">
         <f t="shared" si="2"/>
-        <v>31.49674501956251</v>
+        <v>31.746709098163304</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -18918,7 +18917,7 @@
       </c>
       <c r="E23">
         <f t="shared" si="2"/>
-        <v>32.027113505709238</v>
+        <v>32.266519374903865</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -18938,7 +18937,7 @@
       </c>
       <c r="E24">
         <f t="shared" si="2"/>
-        <v>32.511393350303365</v>
+        <v>32.740167120457009</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -18958,7 +18957,7 @@
       </c>
       <c r="E25">
         <f t="shared" si="2"/>
-        <v>32.953589623283314</v>
+        <v>33.171751867634946</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -18978,7 +18977,7 @@
       </c>
       <c r="E26">
         <f t="shared" si="2"/>
-        <v>33.357359356878661</v>
+        <v>33.565009084090441</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -18998,7 +18997,7 @@
       </c>
       <c r="E27">
         <f t="shared" si="2"/>
-        <v>33.726041789837666</v>
+        <v>33.92334250366924</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -19018,7 +19017,7 @@
       </c>
       <c r="E28">
         <f t="shared" si="2"/>
-        <v>34.062685983453221</v>
+        <v>34.249853586528324</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -19038,7 +19037,7 @@
       </c>
       <c r="E29">
         <f t="shared" si="2"/>
-        <v>34.370076037775853</v>
+        <v>34.547368363004189</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -19058,7 +19057,7 @@
       </c>
       <c r="E30">
         <f t="shared" si="2"/>
-        <v>34.650754116555888</v>
+        <v>34.818461893571047</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -19078,7 +19077,7 @@
       </c>
       <c r="E31">
         <f t="shared" si="2"/>
-        <v>34.907041471334665</v>
+        <v>35.065480556595908</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -19098,7 +19097,7 @@
       </c>
       <c r="E32">
         <f t="shared" si="2"/>
-        <v>35.141057638557257</v>
+        <v>35.290562356795995</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -19118,7 +19117,7 @@
       </c>
       <c r="E33">
         <f t="shared" si="2"/>
-        <v>35.354737968469834</v>
+        <v>35.495655430173279</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -19138,7 +19137,7 @@
       </c>
       <c r="E34">
         <f t="shared" si="2"/>
-        <v>35.549849630768442</v>
+        <v>35.682534905590408</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -19158,7 +19157,7 @@
       </c>
       <c r="E35">
         <f t="shared" si="2"/>
-        <v>35.728006229368319</v>
+        <v>35.852818268929255</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -19178,7 +19177,7 @@
       </c>
       <c r="E36">
         <f t="shared" si="2"/>
-        <v>35.890681147160279</v>
+        <v>36.007979362812179</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -19198,7 +19197,7 @@
       </c>
       <c r="E37">
         <f t="shared" si="2"/>
-        <v>36.039219731117278</v>
+        <v>36.149361143057142</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -19218,7 +19217,7 @@
       </c>
       <c r="E38">
         <f t="shared" si="2"/>
-        <v>36.17485041852396</v>
+        <v>36.278187302276642</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -19238,7 +19237,7 @@
       </c>
       <c r="E39">
         <f t="shared" si="2"/>
-        <v>36.298694896344863</v>
+        <v>36.395572861225567</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -19258,7 +19257,7 @@
       </c>
       <c r="E40">
         <f t="shared" si="2"/>
-        <v>36.411777377750731</v>
+        <v>36.502533819568463</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -19278,7 +19277,7 @@
       </c>
       <c r="E41">
         <f t="shared" si="2"/>
-        <v>36.515033072521405</v>
+        <v>36.59999594959595</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -19298,7 +19297,7 @@
       </c>
       <c r="E42">
         <f t="shared" si="2"/>
-        <v>36.609315921376727</v>
+        <v>36.688802809002013</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -19318,7 +19317,7 @@
       </c>
       <c r="E43">
         <f t="shared" si="2"/>
-        <v>36.695405658199661</v>
+        <v>36.769723042074538</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -19338,7 +19337,7 @@
       </c>
       <c r="E44">
         <f t="shared" si="2"/>
-        <v>36.774014258557223</v>
+        <v>36.843457032492665</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -19358,7 +19357,7 @@
       </c>
       <c r="E45">
         <f t="shared" si="2"/>
-        <v>36.845791827849666</v>
+        <v>36.910642965312562</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -19378,7 +19377,7 @@
       </c>
       <c r="E46">
         <f t="shared" si="2"/>
-        <v>36.911331977783597</v>
+        <v>36.971862350609385</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -19398,7 +19397,7 @@
       </c>
       <c r="E47">
         <f t="shared" si="2"/>
-        <v>36.971176735633513</v>
+        <v>37.027645056583978</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -19418,7 +19417,7 @@
       </c>
       <c r="E48">
         <f t="shared" si="2"/>
-        <v>37.025821026892011</v>
+        <v>37.078473895696952</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -19438,7 +19437,7 @@
       </c>
       <c r="E49">
         <f t="shared" si="2"/>
-        <v>37.075716768380879</v>
+        <v>37.124788803524297</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -19458,7 +19457,7 @@
       </c>
       <c r="E50">
         <f t="shared" si="2"/>
-        <v>37.121276605673806</v>
+        <v>37.166990646503386</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -19478,7 +19477,7 @@
       </c>
       <c r="E51">
         <f t="shared" si="2"/>
-        <v>37.162877325739672</v>
+        <v>37.205444691526452</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -19498,7 +19497,7 @@
       </c>
       <c r="E52">
         <f t="shared" si="2"/>
-        <v>37.200862973029679</v>
+        <v>37.240483767411568</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -19518,7 +19517,7 @@
       </c>
       <c r="E53">
         <f t="shared" si="2"/>
-        <v>37.235547694778624</v>
+        <v>37.272411145614463</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -19538,7 +19537,7 @@
       </c>
       <c r="E54">
         <f t="shared" si="2"/>
-        <v>37.267218339051638</v>
+        <v>37.30150316511444</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -19558,7 +19557,7 @@
       </c>
       <c r="E55">
         <f t="shared" si="2"/>
-        <v>37.296136827022451</v>
+        <v>37.328011624193309</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -19578,7 +19577,7 @@
       </c>
       <c r="E56">
         <f t="shared" si="2"/>
-        <v>37.322542319102403</v>
+        <v>37.352165959808836</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -19598,7 +19597,7 @@
       </c>
       <c r="E57">
         <f t="shared" si="2"/>
-        <v>37.346653192834388</v>
+        <v>37.374175233425682</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -19618,7 +19617,7 @@
       </c>
       <c r="E58">
         <f t="shared" si="2"/>
-        <v>37.368668848909259</v>
+        <v>37.394229940491584</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -19638,7 +19637,7 @@
       </c>
       <c r="E59">
         <f t="shared" si="2"/>
-        <v>37.388771360240639</v>
+        <v>37.412503659220384</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -19658,7 +19657,7 @@
       </c>
       <c r="E60">
         <f t="shared" si="2"/>
-        <v>37.407126977736404</v>
+        <v>37.429154552952305</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -19678,7 +19677,7 @@
       </c>
       <c r="E61">
         <f t="shared" si="2"/>
-        <v>37.423887505219582</v>
+        <v>37.444326739094954</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -19698,7 +19697,7 @@
       </c>
       <c r="E62">
         <f t="shared" si="2"/>
-        <v>37.439191554869744</v>
+        <v>37.458151536493411</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -19718,7 +19717,7 @@
       </c>
       <c r="E63">
         <f t="shared" si="2"/>
-        <v>37.453165693567328</v>
+        <v>37.470748602025807</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -19738,7 +19737,7 @@
       </c>
       <c r="E64">
         <f t="shared" si="2"/>
-        <v>37.465925489621519</v>
+        <v>37.482226966261727</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -19758,7 +19757,7 @@
       </c>
       <c r="E65">
         <f t="shared" si="2"/>
-        <v>37.477576468538217</v>
+        <v>37.492685977147524</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -19778,7 +19777,7 @@
       </c>
       <c r="E66">
         <f t="shared" si="2"/>
-        <v>37.488214985732441</v>
+        <v>37.502216159886196</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -19797,8 +19796,8 @@
         <v>6.5</v>
       </c>
       <c r="E67">
-        <f t="shared" ref="E67:E92" si="5">$G$1*(1-EXP(-D67/$F$1))</f>
-        <v>37.497929023402669</v>
+        <f t="shared" ref="E67:E92" si="5">$G$1*(1-EXP(-D67*$F$1))</f>
+        <v>37.510900000454299</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -19818,7 +19817,7 @@
       </c>
       <c r="E68">
         <f t="shared" si="5"/>
-        <v>37.506798918157344</v>
+        <v>37.518812659537573</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -19838,7 +19837,7 @@
       </c>
       <c r="E69">
         <f t="shared" si="5"/>
-        <v>37.514898025411192</v>
+        <v>37.526022623064307</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -19858,7 +19857,7 @@
       </c>
       <c r="E70">
         <f t="shared" si="5"/>
-        <v>37.522293326045926</v>
+        <v>37.532592294967237</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -19878,7 +19877,7 @@
       </c>
       <c r="E71">
         <f t="shared" si="5"/>
-        <v>37.52904598035262</v>
+        <v>37.538578537304268</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -19898,7 +19897,7 @@
       </c>
       <c r="E72">
         <f t="shared" si="5"/>
-        <v>37.535211833836868</v>
+        <v>37.544033162412966</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -19918,7 +19917,7 @@
       </c>
       <c r="E73">
         <f t="shared" si="5"/>
-        <v>37.540841879069831</v>
+        <v>37.549003381358567</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -19938,7 +19937,7 @@
       </c>
       <c r="E74">
         <f t="shared" si="5"/>
-        <v>37.545982677404751</v>
+        <v>37.553532212556846</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -19958,7 +19957,7 @@
       </c>
       <c r="E75">
         <f t="shared" si="5"/>
-        <v>37.550676744046633</v>
+        <v>37.557658854108652</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -19978,7 +19977,7 @@
       </c>
       <c r="E76">
         <f t="shared" si="5"/>
-        <v>37.554962899659607</v>
+        <v>37.561419023068716</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -19998,7 +19997,7 @@
       </c>
       <c r="E77">
         <f t="shared" si="5"/>
-        <v>37.55887659141991</v>
+        <v>37.564845264585138</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -20018,7 +20017,7 @@
       </c>
       <c r="E78">
         <f t="shared" si="5"/>
-        <v>37.562450186169556</v>
+        <v>37.56796723358535</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -20038,7 +20037,7 @@
       </c>
       <c r="E79">
         <f t="shared" si="5"/>
-        <v>37.565713238095157</v>
+        <v>37.570811951446466</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -20058,7 +20057,7 @@
       </c>
       <c r="E80">
         <f t="shared" si="5"/>
-        <v>37.568692733145689</v>
+        <v>37.57340403987169</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
@@ -20078,7 +20077,7 @@
       </c>
       <c r="E81">
         <f t="shared" si="5"/>
-        <v>37.571413312210481</v>
+        <v>37.575765933996948</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -20098,7 +20097,7 @@
       </c>
       <c r="E82">
         <f t="shared" si="5"/>
-        <v>37.573897474903255</v>
+        <v>37.577918076572274</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -20118,7 +20117,7 @@
       </c>
       <c r="E83">
         <f t="shared" si="5"/>
-        <v>37.576165765637384</v>
+        <v>37.579879094898615</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -20138,7 +20137,7 @@
       </c>
       <c r="E84">
         <f t="shared" si="5"/>
-        <v>37.578236943531458</v>
+        <v>37.581665962051545</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -20158,7 +20157,7 @@
       </c>
       <c r="E85">
         <f t="shared" si="5"/>
-        <v>37.580128137550084</v>
+        <v>37.583294143787185</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -20178,7 +20177,7 @@
       </c>
       <c r="E86">
         <f t="shared" si="5"/>
-        <v>37.581854988163123</v>
+        <v>37.584777732402003</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -20198,7 +20197,7 @@
       </c>
       <c r="E87">
         <f t="shared" si="5"/>
-        <v>37.583431776694795</v>
+        <v>37.586129568704933</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -20218,7 +20217,7 @@
       </c>
       <c r="E88">
         <f t="shared" si="5"/>
-        <v>37.584871543432492</v>
+        <v>37.587361353157632</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
@@ -20238,7 +20237,7 @@
       </c>
       <c r="E89">
         <f t="shared" si="5"/>
-        <v>37.586186195471967</v>
+        <v>37.5884837471447</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -20258,7 +20257,7 @@
       </c>
       <c r="E90">
         <f t="shared" si="5"/>
-        <v>37.587386605190865</v>
+        <v>37.58950646525048</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -20278,7 +20277,7 @@
       </c>
       <c r="E91">
         <f t="shared" si="5"/>
-        <v>37.588482700165031</v>
+        <v>37.590438359341107</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -20298,7 +20297,7 @@
       </c>
       <c r="E92">
         <f t="shared" si="5"/>
-        <v>37.589483545271051</v>
+        <v>37.591287495179451</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>